<commit_message>
Add VAT and gross to Stark MOP annual parser
</commit_message>
<xml_diff>
--- a/test/electricity/bills.annual.mop.stark.xlsx
+++ b/test/electricity/bills.annual.mop.stark.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t xml:space="preserve">Invoice Date</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t xml:space="preserve">Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross</t>
   </si>
   <si>
     <t xml:space="preserve">PS</t>
@@ -174,18 +180,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.34"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -198,21 +204,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B6:I13"/>
+  <dimension ref="B6:K13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -248,19 +256,25 @@
       <c r="I11" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="n">
         <v>1472066139971</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F12" s="4" t="n">
         <v>43252</v>
@@ -273,6 +287,12 @@
       </c>
       <c r="I12" s="0" t="n">
         <v>135.81</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>13.56</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>136.31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,13 +300,13 @@
         <v>1472066139971</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F13" s="4" t="n">
         <v>29738</v>
@@ -299,12 +319,18 @@
       </c>
       <c r="I13" s="0" t="n">
         <v>135.81</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>13.56</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>136.31</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>